<commit_message>
Changed error in file
</commit_message>
<xml_diff>
--- a/Confocal image metrics data.xlsx
+++ b/Confocal image metrics data.xlsx
@@ -1,35 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Richard\Jorge\2024_02_07_ImageData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix_9ny56v1\Python\Copenhagen\OrganoCellQuant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A4D133-69A6-4365-81A5-7C9D30D33279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E293C6B-1554-492F-9003-52FAA9D04D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10815" yWindow="5655" windowWidth="43200" windowHeight="17145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -981,7 +970,7 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -997,9 +986,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1037,7 +1026,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1143,7 +1132,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1285,7 +1274,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1295,12 +1284,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V186"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C183" sqref="C183"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I170" sqref="I170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="32.28515625" customWidth="1"/>
     <col min="8" max="8" width="56.5703125" customWidth="1"/>
@@ -6259,7 +6248,7 @@
         <v>256</v>
       </c>
       <c r="I164" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>